<commit_message>
updated tumor size measurements
</commit_message>
<xml_diff>
--- a/data/tumor-size/AOT00054521-mimic22/AOT00054521_mimic22_tumor-size.xlsx
+++ b/data/tumor-size/AOT00054521-mimic22/AOT00054521_mimic22_tumor-size.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27424"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osumc-my.sharepoint.com/personal/wil407_osumc_edu/Documents/BuckeyeBox Data/mimic/data/AOT00054521-mimic22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="702" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE565E01-035A-44A5-8A38-172BEE3ADF32}"/>
+  <xr:revisionPtr revIDLastSave="730" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{105E8687-9A8F-4776-A368-42F414C4D04B}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,10 +175,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,11 +476,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B161" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174:XFD174"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="K226" sqref="K226"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -497,7 +493,7 @@
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>45287</v>
       </c>
@@ -546,7 +542,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>45287</v>
       </c>
@@ -560,7 +556,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>45287</v>
       </c>
@@ -574,7 +570,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>45287</v>
       </c>
@@ -588,7 +584,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>45287</v>
       </c>
@@ -602,7 +598,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>45287</v>
       </c>
@@ -616,7 +612,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>45287</v>
       </c>
@@ -630,7 +626,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>45287</v>
       </c>
@@ -644,7 +640,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>45287</v>
       </c>
@@ -658,7 +654,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>45287</v>
       </c>
@@ -672,7 +668,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>45287</v>
       </c>
@@ -686,7 +682,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>45287</v>
       </c>
@@ -700,7 +696,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>45287</v>
       </c>
@@ -714,7 +710,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>45287</v>
       </c>
@@ -728,7 +724,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>45287</v>
       </c>
@@ -742,7 +738,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>45287</v>
       </c>
@@ -756,7 +752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>45287</v>
       </c>
@@ -770,7 +766,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>45287</v>
       </c>
@@ -784,7 +780,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>45287</v>
       </c>
@@ -798,7 +794,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="2">
         <v>45287</v>
       </c>
@@ -812,7 +808,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>45287</v>
       </c>
@@ -826,7 +822,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>45287</v>
       </c>
@@ -840,7 +836,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>45287</v>
       </c>
@@ -854,7 +850,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="2">
         <v>45287</v>
       </c>
@@ -868,7 +864,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>45309</v>
       </c>
@@ -885,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>45309</v>
       </c>
@@ -902,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>45309</v>
       </c>
@@ -919,7 +915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="2">
         <v>45309</v>
       </c>
@@ -936,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="2">
         <v>45309</v>
       </c>
@@ -953,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>45309</v>
       </c>
@@ -970,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="2">
         <v>45309</v>
       </c>
@@ -987,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="2">
         <v>45309</v>
       </c>
@@ -1004,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="2">
         <v>45309</v>
       </c>
@@ -1021,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="2">
         <v>45309</v>
       </c>
@@ -1038,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="2">
         <v>45309</v>
       </c>
@@ -1055,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="2">
         <v>45309</v>
       </c>
@@ -1072,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="2">
         <v>45309</v>
       </c>
@@ -1089,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="2">
         <v>45309</v>
       </c>
@@ -1106,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="2">
         <v>45309</v>
       </c>
@@ -1123,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="2">
         <v>45309</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="2">
         <v>45309</v>
       </c>
@@ -1157,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="2">
         <v>45309</v>
       </c>
@@ -1174,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="2">
         <v>45309</v>
       </c>
@@ -1191,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="2">
         <v>45309</v>
       </c>
@@ -1208,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="2">
         <v>45309</v>
       </c>
@@ -1225,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="2">
         <v>45309</v>
       </c>
@@ -1242,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="2">
         <v>45309</v>
       </c>
@@ -1259,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="2">
         <v>45309</v>
       </c>
@@ -1276,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="2">
         <v>45313</v>
       </c>
@@ -1296,7 +1292,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="2">
         <v>45313</v>
       </c>
@@ -1316,7 +1312,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="2">
         <v>45313</v>
       </c>
@@ -1336,7 +1332,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="2">
         <v>45313</v>
       </c>
@@ -1356,7 +1352,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="2">
         <v>45313</v>
       </c>
@@ -1376,7 +1372,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="2">
         <v>45313</v>
       </c>
@@ -1396,7 +1392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="2">
         <v>45313</v>
       </c>
@@ -1416,7 +1412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="2">
         <v>45313</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="2">
         <v>45313</v>
       </c>
@@ -1456,7 +1452,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="2">
         <v>45313</v>
       </c>
@@ -1476,7 +1472,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="2">
         <v>45313</v>
       </c>
@@ -1496,7 +1492,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="2">
         <v>45313</v>
       </c>
@@ -1516,7 +1512,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="2">
         <v>45313</v>
       </c>
@@ -1536,7 +1532,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="2">
         <v>45313</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="2">
         <v>45313</v>
       </c>
@@ -1576,7 +1572,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" s="2">
         <v>45313</v>
       </c>
@@ -1596,7 +1592,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="A66" s="2">
         <v>45313</v>
       </c>
@@ -1616,7 +1612,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="A67" s="2">
         <v>45313</v>
       </c>
@@ -1636,7 +1632,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="A68" s="2">
         <v>45313</v>
       </c>
@@ -1656,7 +1652,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9">
       <c r="A69" s="2">
         <v>45313</v>
       </c>
@@ -1676,7 +1672,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9">
       <c r="A70" s="2">
         <v>45313</v>
       </c>
@@ -1696,7 +1692,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9">
       <c r="A71" s="2">
         <v>45313</v>
       </c>
@@ -1716,7 +1712,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9">
       <c r="A72" s="2">
         <v>45313</v>
       </c>
@@ -1736,7 +1732,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9">
       <c r="A73" s="2">
         <v>45313</v>
       </c>
@@ -1756,7 +1752,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9">
       <c r="A74" s="2">
         <v>45315</v>
       </c>
@@ -1782,7 +1778,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9">
       <c r="A75" s="2">
         <v>45315</v>
       </c>
@@ -1808,7 +1804,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9">
       <c r="A76" s="2">
         <v>45315</v>
       </c>
@@ -1834,7 +1830,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9">
       <c r="A77" s="2">
         <v>45315</v>
       </c>
@@ -1860,7 +1856,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9">
       <c r="A78" s="2">
         <v>45315</v>
       </c>
@@ -1886,7 +1882,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" s="2">
         <v>45315</v>
       </c>
@@ -1912,7 +1908,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="2">
         <v>45315</v>
       </c>
@@ -1938,7 +1934,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9">
       <c r="A81" s="2">
         <v>45315</v>
       </c>
@@ -1964,7 +1960,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9">
       <c r="A82" s="2">
         <v>45315</v>
       </c>
@@ -1990,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9">
       <c r="A83" s="2">
         <v>45315</v>
       </c>
@@ -2016,7 +2012,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9">
       <c r="A84" s="2">
         <v>45315</v>
       </c>
@@ -2042,7 +2038,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9">
       <c r="A85" s="2">
         <v>45315</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9">
       <c r="A86" s="2">
         <v>45315</v>
       </c>
@@ -2094,7 +2090,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9">
       <c r="A87" s="2">
         <v>45315</v>
       </c>
@@ -2120,7 +2116,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9">
       <c r="A88" s="2">
         <v>45315</v>
       </c>
@@ -2146,7 +2142,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9">
       <c r="A89" s="2">
         <v>45315</v>
       </c>
@@ -2172,7 +2168,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9">
       <c r="A90" s="2">
         <v>45315</v>
       </c>
@@ -2198,7 +2194,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9">
       <c r="A91" s="2">
         <v>45315</v>
       </c>
@@ -2224,7 +2220,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9">
       <c r="A92" s="2">
         <v>45315</v>
       </c>
@@ -2250,7 +2246,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9">
       <c r="A93" s="2">
         <v>45315</v>
       </c>
@@ -2276,7 +2272,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9">
       <c r="A94" s="2">
         <v>45315</v>
       </c>
@@ -2302,7 +2298,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9">
       <c r="A95" s="2">
         <v>45315</v>
       </c>
@@ -2328,7 +2324,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9">
       <c r="A96" s="2">
         <v>45315</v>
       </c>
@@ -2354,7 +2350,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9">
       <c r="A97" s="2">
         <v>45315</v>
       </c>
@@ -2380,7 +2376,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9">
       <c r="A98" s="2">
         <v>45318</v>
       </c>
@@ -2406,7 +2402,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9">
       <c r="A99" s="2">
         <v>45318</v>
       </c>
@@ -2432,7 +2428,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9">
       <c r="A100" s="2">
         <v>45318</v>
       </c>
@@ -2458,7 +2454,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9">
       <c r="A101" s="2">
         <v>45318</v>
       </c>
@@ -2484,7 +2480,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9">
       <c r="A102" s="2">
         <v>45318</v>
       </c>
@@ -2510,7 +2506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9">
       <c r="A103" s="2">
         <v>45318</v>
       </c>
@@ -2536,7 +2532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9">
       <c r="A104" s="2">
         <v>45318</v>
       </c>
@@ -2562,7 +2558,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9">
       <c r="A105" s="2">
         <v>45318</v>
       </c>
@@ -2588,7 +2584,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9">
       <c r="A106" s="2">
         <v>45318</v>
       </c>
@@ -2614,7 +2610,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9">
       <c r="A107" s="2">
         <v>45318</v>
       </c>
@@ -2640,7 +2636,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9">
       <c r="A108" s="2">
         <v>45318</v>
       </c>
@@ -2666,7 +2662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9">
       <c r="A109" s="2">
         <v>45318</v>
       </c>
@@ -2692,7 +2688,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9">
       <c r="A110" s="2">
         <v>45318</v>
       </c>
@@ -2718,7 +2714,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9">
       <c r="A111" s="2">
         <v>45318</v>
       </c>
@@ -2744,7 +2740,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9">
       <c r="A112" s="2">
         <v>45318</v>
       </c>
@@ -2770,7 +2766,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9">
       <c r="A113" s="2">
         <v>45318</v>
       </c>
@@ -2796,7 +2792,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9">
       <c r="A114" s="2">
         <v>45318</v>
       </c>
@@ -2822,7 +2818,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9">
       <c r="A115" s="2">
         <v>45318</v>
       </c>
@@ -2848,7 +2844,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9">
       <c r="A116" s="2">
         <v>45318</v>
       </c>
@@ -2874,7 +2870,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9">
       <c r="A117" s="2">
         <v>45318</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9">
       <c r="A118" s="2">
         <v>45318</v>
       </c>
@@ -2926,7 +2922,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9">
       <c r="A119" s="2">
         <v>45318</v>
       </c>
@@ -2952,7 +2948,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9">
       <c r="A120" s="2">
         <v>45318</v>
       </c>
@@ -2978,7 +2974,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9">
       <c r="A121" s="2">
         <v>45318</v>
       </c>
@@ -3004,7 +3000,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9">
       <c r="A122" s="2">
         <v>45318</v>
       </c>
@@ -3030,7 +3026,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9">
       <c r="A123" s="2">
         <v>45321</v>
       </c>
@@ -3056,7 +3052,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9">
       <c r="A124" s="2">
         <v>45321</v>
       </c>
@@ -3082,7 +3078,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9">
       <c r="A125" s="2">
         <v>45321</v>
       </c>
@@ -3108,7 +3104,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9">
       <c r="A126" s="2">
         <v>45321</v>
       </c>
@@ -3134,7 +3130,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9">
       <c r="A127" s="2">
         <v>45321</v>
       </c>
@@ -3160,7 +3156,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9">
       <c r="A128" s="2">
         <v>45321</v>
       </c>
@@ -3186,7 +3182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9">
       <c r="A129" s="2">
         <v>45321</v>
       </c>
@@ -3212,7 +3208,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9">
       <c r="A130" s="2">
         <v>45321</v>
       </c>
@@ -3238,7 +3234,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9">
       <c r="A131" s="2">
         <v>45321</v>
       </c>
@@ -3264,7 +3260,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9">
       <c r="A132" s="2">
         <v>45321</v>
       </c>
@@ -3290,7 +3286,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9">
       <c r="A133" s="2">
         <v>45321</v>
       </c>
@@ -3316,7 +3312,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9">
       <c r="A134" s="2">
         <v>45321</v>
       </c>
@@ -3342,7 +3338,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9">
       <c r="A135" s="2">
         <v>45321</v>
       </c>
@@ -3368,7 +3364,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9">
       <c r="A136" s="2">
         <v>45321</v>
       </c>
@@ -3394,7 +3390,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9">
       <c r="A137" s="2">
         <v>45321</v>
       </c>
@@ -3420,7 +3416,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9">
       <c r="A138" s="2">
         <v>45321</v>
       </c>
@@ -3446,7 +3442,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9">
       <c r="A139" s="2">
         <v>45321</v>
       </c>
@@ -3472,7 +3468,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9">
       <c r="A140" s="2">
         <v>45321</v>
       </c>
@@ -3498,7 +3494,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9">
       <c r="A141" s="2">
         <v>45321</v>
       </c>
@@ -3524,7 +3520,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9">
       <c r="A142" s="2">
         <v>45321</v>
       </c>
@@ -3550,7 +3546,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9">
       <c r="A143" s="2">
         <v>45321</v>
       </c>
@@ -3576,7 +3572,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9">
       <c r="A144" s="2">
         <v>45321</v>
       </c>
@@ -3602,7 +3598,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9">
       <c r="A145" s="2">
         <v>45321</v>
       </c>
@@ -3628,7 +3624,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9">
       <c r="A146" s="2">
         <v>45321</v>
       </c>
@@ -3654,7 +3650,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9">
       <c r="A147" s="2">
         <v>45321</v>
       </c>
@@ -3680,7 +3676,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9">
       <c r="A148" s="2">
         <v>45321</v>
       </c>
@@ -3706,7 +3702,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9">
       <c r="A149" s="2">
         <v>45324</v>
       </c>
@@ -3732,7 +3728,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9">
       <c r="A150" s="2">
         <v>45324</v>
       </c>
@@ -3758,7 +3754,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9">
       <c r="A151" s="2">
         <v>45324</v>
       </c>
@@ -3784,7 +3780,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9">
       <c r="A152" s="2">
         <v>45324</v>
       </c>
@@ -3810,7 +3806,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9">
       <c r="A153" s="2">
         <v>45324</v>
       </c>
@@ -3836,7 +3832,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9">
       <c r="A154" s="2">
         <v>45324</v>
       </c>
@@ -3862,7 +3858,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9">
       <c r="A155" s="2">
         <v>45324</v>
       </c>
@@ -3888,7 +3884,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9">
       <c r="A156" s="2">
         <v>45324</v>
       </c>
@@ -3914,7 +3910,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9">
       <c r="A157" s="2">
         <v>45324</v>
       </c>
@@ -3940,7 +3936,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9">
       <c r="A158" s="2">
         <v>45324</v>
       </c>
@@ -3966,7 +3962,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9">
       <c r="A159" s="2">
         <v>45324</v>
       </c>
@@ -3992,7 +3988,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9">
       <c r="A160" s="2">
         <v>45324</v>
       </c>
@@ -4018,7 +4014,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9">
       <c r="A161" s="2">
         <v>45324</v>
       </c>
@@ -4044,7 +4040,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9">
       <c r="A162" s="2">
         <v>45324</v>
       </c>
@@ -4070,7 +4066,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9">
       <c r="A163" s="2">
         <v>45324</v>
       </c>
@@ -4096,7 +4092,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9">
       <c r="A164" s="2">
         <v>45324</v>
       </c>
@@ -4122,7 +4118,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9">
       <c r="A165" s="2">
         <v>45324</v>
       </c>
@@ -4148,7 +4144,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9">
       <c r="A166" s="2">
         <v>45324</v>
       </c>
@@ -4174,7 +4170,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9">
       <c r="A167" s="2">
         <v>45324</v>
       </c>
@@ -4200,7 +4196,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9">
       <c r="A168" s="2">
         <v>45324</v>
       </c>
@@ -4226,7 +4222,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9">
       <c r="A169" s="2">
         <v>45324</v>
       </c>
@@ -4252,7 +4248,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9">
       <c r="A170" s="2">
         <v>45324</v>
       </c>
@@ -4278,7 +4274,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9">
       <c r="A171" s="2">
         <v>45324</v>
       </c>
@@ -4304,7 +4300,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9">
       <c r="A172" s="2">
         <v>45324</v>
       </c>
@@ -4330,7 +4326,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9">
       <c r="A173" s="2">
         <v>45324</v>
       </c>
@@ -4356,7 +4352,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9">
       <c r="A174" s="2">
         <v>45324</v>
       </c>
@@ -4382,7 +4378,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9">
       <c r="A175" s="2">
         <v>45327</v>
       </c>
@@ -4408,7 +4404,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9">
       <c r="A176" s="2">
         <v>45327</v>
       </c>
@@ -4434,7 +4430,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9">
       <c r="A177" s="2">
         <v>45327</v>
       </c>
@@ -4460,7 +4456,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9">
       <c r="A178" s="2">
         <v>45327</v>
       </c>
@@ -4480,13 +4476,13 @@
         <v>1</v>
       </c>
       <c r="H178">
-        <v>10.5</v>
+        <v>13.1</v>
       </c>
       <c r="I178">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9">
       <c r="A179" s="2">
         <v>45327</v>
       </c>
@@ -4506,13 +4502,13 @@
         <v>1</v>
       </c>
       <c r="H179">
-        <v>13.1</v>
+        <v>10.5</v>
       </c>
       <c r="I179">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9">
       <c r="A180" s="2">
         <v>45327</v>
       </c>
@@ -4532,13 +4528,13 @@
         <v>2</v>
       </c>
       <c r="H180">
-        <v>13.8</v>
+        <v>13.1</v>
       </c>
       <c r="I180">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9">
       <c r="A181" s="2">
         <v>45327</v>
       </c>
@@ -4558,13 +4554,13 @@
         <v>1</v>
       </c>
       <c r="H181">
-        <v>13.1</v>
+        <v>13.8</v>
       </c>
       <c r="I181">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9">
       <c r="A182" s="2">
         <v>45327</v>
       </c>
@@ -4590,7 +4586,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9">
       <c r="A183" s="2">
         <v>45327</v>
       </c>
@@ -4616,7 +4612,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9">
       <c r="A184" s="2">
         <v>45327</v>
       </c>
@@ -4642,7 +4638,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9">
       <c r="A185" s="2">
         <v>45327</v>
       </c>
@@ -4668,7 +4664,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9">
       <c r="A186" s="2">
         <v>45327</v>
       </c>
@@ -4694,7 +4690,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9">
       <c r="A187" s="2">
         <v>45327</v>
       </c>
@@ -4720,7 +4716,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9">
       <c r="A188" s="2">
         <v>45327</v>
       </c>
@@ -4746,7 +4742,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9">
       <c r="A189" s="2">
         <v>45327</v>
       </c>
@@ -4772,7 +4768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9">
       <c r="A190" s="2">
         <v>45327</v>
       </c>
@@ -4798,7 +4794,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9">
       <c r="A191" s="2">
         <v>45327</v>
       </c>
@@ -4824,7 +4820,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9">
       <c r="A192" s="2">
         <v>45327</v>
       </c>
@@ -4850,7 +4846,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="2">
         <v>45327</v>
       </c>
@@ -4876,7 +4872,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="2">
         <v>45327</v>
       </c>
@@ -4902,7 +4898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="2">
         <v>45327</v>
       </c>
@@ -4928,7 +4924,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="2">
         <v>45327</v>
       </c>
@@ -4954,7 +4950,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="2">
         <v>45327</v>
       </c>
@@ -4980,7 +4976,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="2">
         <v>45327</v>
       </c>
@@ -5006,7 +5002,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="2">
         <v>45327</v>
       </c>
@@ -5032,7 +5028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="2">
         <v>45327</v>
       </c>
@@ -5058,7 +5054,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="2">
         <v>45330</v>
       </c>
@@ -5090,7 +5086,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="2">
         <v>45330</v>
       </c>
@@ -5122,7 +5118,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="2">
         <v>45330</v>
       </c>
@@ -5154,7 +5150,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="2">
         <v>45330</v>
       </c>
@@ -5186,7 +5182,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="2">
         <v>45330</v>
       </c>
@@ -5218,7 +5214,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="2">
         <v>45330</v>
       </c>
@@ -5250,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="2">
         <v>45330</v>
       </c>
@@ -5282,7 +5278,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="2">
         <v>45330</v>
       </c>
@@ -5314,7 +5310,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="2">
         <v>45330</v>
       </c>
@@ -5346,7 +5342,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="2">
         <v>45330</v>
       </c>
@@ -5378,7 +5374,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="2">
         <v>45330</v>
       </c>
@@ -5410,7 +5406,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="2">
         <v>45330</v>
       </c>
@@ -5442,7 +5438,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="2">
         <v>45330</v>
       </c>
@@ -5474,7 +5470,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="2">
         <v>45330</v>
       </c>
@@ -5506,7 +5502,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="2">
         <v>45330</v>
       </c>
@@ -5538,7 +5534,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="2">
         <v>45330</v>
       </c>
@@ -5570,7 +5566,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="2">
         <v>45330</v>
       </c>
@@ -5602,7 +5598,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="2">
         <v>45330</v>
       </c>
@@ -5634,7 +5630,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="2">
         <v>45330</v>
       </c>
@@ -5666,7 +5662,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="2">
         <v>45330</v>
       </c>
@@ -5698,7 +5694,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="2">
         <v>45330</v>
       </c>
@@ -5730,7 +5726,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="2">
         <v>45330</v>
       </c>
@@ -5762,7 +5758,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="2">
         <v>45330</v>
       </c>
@@ -5794,7 +5790,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="2">
         <v>45330</v>
       </c>
@@ -5826,7 +5822,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="2">
         <v>45330</v>
       </c>

</xml_diff>